<commit_message>
make code per add item to each zone start highamper by 1 start lowamper by 17
</commit_message>
<xml_diff>
--- a/flask-backend/List.xlsx
+++ b/flask-backend/List.xlsx
@@ -1,72 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rose\Desktop\Smart Home\RestfulFlaskPythonReact\flask-backend\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B59CF2-49F0-4EA6-AB51-9AC89F0B5F79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="List" sheetId="1" r:id="rId1"/>
+    <sheet name="LowAmper" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="HighAmper" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LowAmper'!$A$1:$G$100</definedName>
+  </definedNames>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t xml:space="preserve">code </t>
-  </si>
-  <si>
-    <t>zone id</t>
-  </si>
-  <si>
-    <t>item id</t>
-  </si>
-  <si>
-    <t>item name</t>
-  </si>
-  <si>
-    <t>item group</t>
-  </si>
-  <si>
-    <t>zone name</t>
-  </si>
-  <si>
-    <t>speed type</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -84,28 +48,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -371,88 +320,362 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G216"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="A2:I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">code </t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>zone id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>zone name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>item id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>item name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>item group</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>speed type</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>34</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>TV Room</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>iugyop</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Lamp</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>35</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>TV Room</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>iugyop</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Socket</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>36</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>TV Room</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>iugyop</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Curtain</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>37</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>TV Room</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>4</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>iugyop</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Aircondition</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Slow</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>-1</v>
+      </c>
+      <c r="B100" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C100" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D100" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G100" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G100"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I11" sqref="A2:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">code </t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>zone id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>zone name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>item id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>item name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>item group</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>speed type</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>TV Room</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>iugyop</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Aircondition</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TV Room</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>6</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A212" s="1">
-        <v>111</v>
-      </c>
-      <c r="B212" s="1">
-        <v>222</v>
-      </c>
-      <c r="D212" s="1">
-        <v>333</v>
-      </c>
-      <c r="E212" s="1">
-        <v>444</v>
-      </c>
-      <c r="F212" s="1">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" s="1">
-        <v>11</v>
-      </c>
-      <c r="B213" s="1">
-        <v>22</v>
-      </c>
-      <c r="D213" s="1">
-        <v>33</v>
-      </c>
-      <c r="E213" s="1">
-        <v>44</v>
-      </c>
-      <c r="F213" s="1">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F216" s="1">
-        <v>2</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>iugyop</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Aircondition</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Fast</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>-1</v>
+      </c>
+      <c r="B50" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C50" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D50" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
debug some error when send code of item to electronic board
in react should edit lowercase naming variable
</commit_message>
<xml_diff>
--- a/flask-backend/List.xlsx
+++ b/flask-backend/List.xlsx
@@ -328,7 +328,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="A2:I14"/>
+      <selection activeCell="J14" sqref="A14:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -388,7 +388,7 @@
     <row r="17"/>
     <row r="18">
       <c r="A18" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B18" t="n">
         <v>1</v>
@@ -403,7 +403,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>iugyop</t>
+          <t>lamp-1</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -419,27 +419,27 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B19" t="n">
+        <v>9</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>اتاق 3</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
         <v>1</v>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>TV Room</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>2</v>
-      </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>iugyop</t>
+          <t>لوستر</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Socket</t>
+          <t>Lamp</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -450,22 +450,22 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>TV Room</t>
+          <t>اتاق 3</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>iugyop</t>
+          <t>راست</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -481,30 +481,61 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>TV Room</t>
+          <t>اتاق 3</t>
         </is>
       </c>
       <c r="D21" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>چپ</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Curtain</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>22</v>
+      </c>
+      <c r="B22" t="n">
+        <v>9</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>اتاق 3</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
         <v>4</v>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>iugyop</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>کولر 3</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
         <is>
           <t>Aircondition</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>Slow</t>
         </is>
@@ -548,7 +579,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="A2:I11"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -595,11 +626,11 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>TV Room</t>
+          <t>اتاق 3</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -607,7 +638,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>iugyop</t>
+          <t>کولر 3</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -626,11 +657,11 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>TV Room</t>
+          <t>اتاق 3</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -638,7 +669,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>iugyop</t>
+          <t>کولر 3</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">

</xml_diff>